<commit_message>
Beat processing from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/template/customers_template.xlsx
+++ b/src/main/resources/template/customers_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Beat</t>
+  </si>
+  <si>
+    <t>Beat Name</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +120,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,12 +157,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6:Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,119 +476,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="2"/>
+      <c r="Z2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="2:26" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:N1"/>
-    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="O1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>